<commit_message>
Spalte "Betrag" mit Multiplikation ergänzt
</commit_message>
<xml_diff>
--- a/Projekt/Mitarbeiterzeiten/KL/MA_KL.xlsx
+++ b/Projekt/Mitarbeiterzeiten/KL/MA_KL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UBXGitHub\HtmXRechnung\Projekt\Mitarbeiterzeiten\KL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46543BAA-38CD-49D2-A708-FCDF5020B8FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4890B5A-B757-4F0E-AC6E-61A6ADA872CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="870" windowWidth="26460" windowHeight="17505" tabRatio="373" firstSheet="1" activeTab="1" xr2:uid="{5A353484-0E68-4912-BD2B-362C94CA2B03}"/>
+    <workbookView xWindow="1560" yWindow="1305" windowWidth="32595" windowHeight="17505" tabRatio="373" firstSheet="1" activeTab="1" xr2:uid="{5A353484-0E68-4912-BD2B-362C94CA2B03}"/>
   </bookViews>
   <sheets>
     <sheet name="Makros" sheetId="29" state="veryHidden" r:id="rId1"/>

</xml_diff>